<commit_message>
Put all plotting code for sensitivity analysis in plots.py
</commit_message>
<xml_diff>
--- a/solutions/vrp_solution_test_case_6.xlsx
+++ b/solutions/vrp_solution_test_case_6.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B305"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Is job 1 predecessor of job 1?</t>
+          <t>Is job z2 predecessor of job z2?</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -458,17 +458,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Is job 1 predecessor of job 2?</t>
+          <t>Is job z2 predecessor of job 1?</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Is job 1 predecessor of job 3?</t>
+          <t>Is job z2 predecessor of job 2?</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -478,7 +478,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Is job 1 predecessor of job z1?</t>
+          <t>Is job z2 predecessor of job 3?</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -488,7 +488,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Is job 1 predecessor of job s1?</t>
+          <t>Is job z2 predecessor of job 4?</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -498,7 +498,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Is job 2 predecessor of job 1?</t>
+          <t>Is job z2 predecessor of job 5?</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -508,7 +508,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Is job 2 predecessor of job 2?</t>
+          <t>Is job z2 predecessor of job 6?</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -518,17 +518,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Is job 2 predecessor of job 3?</t>
+          <t>Is job z2 predecessor of job 7?</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Is job 2 predecessor of job z1?</t>
+          <t>Is job z2 predecessor of job 8?</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -538,7 +538,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Is job 2 predecessor of job s1?</t>
+          <t>Is job z2 predecessor of job 9?</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -548,7 +548,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Is job 3 predecessor of job 1?</t>
+          <t>Is job z2 predecessor of job 10?</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -558,7 +558,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Is job 3 predecessor of job 2?</t>
+          <t>Is job z2 predecessor of job 11?</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -568,7 +568,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Is job 3 predecessor of job 3?</t>
+          <t>Is job z2 predecessor of job 12?</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -578,27 +578,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Is job 3 predecessor of job z1?</t>
+          <t>Is job z2 predecessor of job z1?</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Is job 3 predecessor of job s1?</t>
+          <t>Is job z2 predecessor of job s1?</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Is job z1 predecessor of job 1?</t>
+          <t>Is job z2 predecessor of job s2?</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -608,7 +608,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Is job z1 predecessor of job 2?</t>
+          <t>Is job 1 predecessor of job z2?</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -618,7 +618,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Is job z1 predecessor of job 3?</t>
+          <t>Is job 1 predecessor of job 1?</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -628,7 +628,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Is job z1 predecessor of job z1?</t>
+          <t>Is job 1 predecessor of job 2?</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -638,27 +638,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Is job z1 predecessor of job s1?</t>
+          <t>Is job 1 predecessor of job 3?</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Is job s1 predecessor of job 1?</t>
+          <t>Is job 1 predecessor of job 4?</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Is job s1 predecessor of job 2?</t>
+          <t>Is job 1 predecessor of job 5?</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -668,7 +668,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Is job s1 predecessor of job 3?</t>
+          <t>Is job 1 predecessor of job 6?</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -678,17 +678,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Is job s1 predecessor of job z1?</t>
+          <t>Is job 1 predecessor of job 7?</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Is job s1 predecessor of job s1?</t>
+          <t>Is job 1 predecessor of job 8?</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -698,57 +698,57 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Job 1 is executed by machine:</t>
+          <t>Is job 1 predecessor of job 9?</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Job 2 is executed by machine:</t>
+          <t>Is job 1 predecessor of job 10?</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Job 3 is executed by machine:</t>
+          <t>Is job 1 predecessor of job 11?</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Job z1 is executed by machine:</t>
+          <t>Is job 1 predecessor of job 12?</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Job s1 is executed by machine:</t>
+          <t>Is job 1 predecessor of job z1?</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Job 1 is executed on day:</t>
+          <t>Is job 1 predecessor of job s1?</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -758,37 +758,37 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Job 2 is executed on day:</t>
+          <t>Is job 1 predecessor of job s2?</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Job 3 is executed on day:</t>
+          <t>Is job 2 predecessor of job z2?</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Job z1 is executed on day:</t>
+          <t>Is job 2 predecessor of job 1?</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Job s1 is executed on day:</t>
+          <t>Is job 2 predecessor of job 2?</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -798,17 +798,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Job 1 is executed on minute:</t>
+          <t>Is job 2 predecessor of job 3?</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Job 2 is executed on minute:</t>
+          <t>Is job 2 predecessor of job 4?</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -818,7 +818,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Job 3 is executed on minute:</t>
+          <t>Is job 2 predecessor of job 5?</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -828,20 +828,2660 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Job z1 is executed on minute:</t>
+          <t>Is job 2 predecessor of job 6?</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>480</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>Is job 2 predecessor of job 7?</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Is job 2 predecessor of job 8?</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Is job 2 predecessor of job 9?</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Is job 2 predecessor of job 10?</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Is job 2 predecessor of job 11?</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Is job 2 predecessor of job 12?</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Is job 2 predecessor of job z1?</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Is job 2 predecessor of job s1?</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Is job 2 predecessor of job s2?</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Is job 3 predecessor of job z2?</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Is job 3 predecessor of job 1?</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Is job 3 predecessor of job 2?</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Is job 3 predecessor of job 3?</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Is job 3 predecessor of job 4?</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Is job 3 predecessor of job 5?</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Is job 3 predecessor of job 6?</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Is job 3 predecessor of job 7?</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Is job 3 predecessor of job 8?</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Is job 3 predecessor of job 9?</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Is job 3 predecessor of job 10?</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Is job 3 predecessor of job 11?</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Is job 3 predecessor of job 12?</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Is job 3 predecessor of job z1?</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Is job 3 predecessor of job s1?</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Is job 3 predecessor of job s2?</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Is job 4 predecessor of job z2?</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Is job 4 predecessor of job 1?</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Is job 4 predecessor of job 2?</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Is job 4 predecessor of job 3?</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Is job 4 predecessor of job 4?</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Is job 4 predecessor of job 5?</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Is job 4 predecessor of job 6?</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Is job 4 predecessor of job 7?</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Is job 4 predecessor of job 8?</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Is job 4 predecessor of job 9?</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Is job 4 predecessor of job 10?</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Is job 4 predecessor of job 11?</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Is job 4 predecessor of job 12?</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Is job 4 predecessor of job z1?</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Is job 4 predecessor of job s1?</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Is job 4 predecessor of job s2?</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Is job 5 predecessor of job z2?</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Is job 5 predecessor of job 1?</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Is job 5 predecessor of job 2?</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Is job 5 predecessor of job 3?</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Is job 5 predecessor of job 4?</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Is job 5 predecessor of job 5?</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Is job 5 predecessor of job 6?</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Is job 5 predecessor of job 7?</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Is job 5 predecessor of job 8?</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Is job 5 predecessor of job 9?</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Is job 5 predecessor of job 10?</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Is job 5 predecessor of job 11?</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Is job 5 predecessor of job 12?</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Is job 5 predecessor of job z1?</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Is job 5 predecessor of job s1?</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Is job 5 predecessor of job s2?</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Is job 6 predecessor of job z2?</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Is job 6 predecessor of job 1?</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Is job 6 predecessor of job 2?</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Is job 6 predecessor of job 3?</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Is job 6 predecessor of job 4?</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Is job 6 predecessor of job 5?</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Is job 6 predecessor of job 6?</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Is job 6 predecessor of job 7?</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Is job 6 predecessor of job 8?</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Is job 6 predecessor of job 9?</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Is job 6 predecessor of job 10?</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Is job 6 predecessor of job 11?</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Is job 6 predecessor of job 12?</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Is job 6 predecessor of job z1?</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Is job 6 predecessor of job s1?</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Is job 6 predecessor of job s2?</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Is job 7 predecessor of job z2?</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Is job 7 predecessor of job 1?</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Is job 7 predecessor of job 2?</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Is job 7 predecessor of job 3?</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Is job 7 predecessor of job 4?</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Is job 7 predecessor of job 5?</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Is job 7 predecessor of job 6?</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Is job 7 predecessor of job 7?</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Is job 7 predecessor of job 8?</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Is job 7 predecessor of job 9?</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Is job 7 predecessor of job 10?</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Is job 7 predecessor of job 11?</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Is job 7 predecessor of job 12?</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Is job 7 predecessor of job z1?</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Is job 7 predecessor of job s1?</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Is job 7 predecessor of job s2?</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Is job 8 predecessor of job z2?</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Is job 8 predecessor of job 1?</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Is job 8 predecessor of job 2?</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Is job 8 predecessor of job 3?</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Is job 8 predecessor of job 4?</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Is job 8 predecessor of job 5?</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Is job 8 predecessor of job 6?</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Is job 8 predecessor of job 7?</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Is job 8 predecessor of job 8?</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Is job 8 predecessor of job 9?</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Is job 8 predecessor of job 10?</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Is job 8 predecessor of job 11?</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Is job 8 predecessor of job 12?</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Is job 8 predecessor of job z1?</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Is job 8 predecessor of job s1?</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Is job 8 predecessor of job s2?</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Is job 9 predecessor of job z2?</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Is job 9 predecessor of job 1?</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Is job 9 predecessor of job 2?</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Is job 9 predecessor of job 3?</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Is job 9 predecessor of job 4?</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Is job 9 predecessor of job 5?</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Is job 9 predecessor of job 6?</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Is job 9 predecessor of job 7?</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Is job 9 predecessor of job 8?</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Is job 9 predecessor of job 9?</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Is job 9 predecessor of job 10?</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Is job 9 predecessor of job 11?</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>Is job 9 predecessor of job 12?</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>Is job 9 predecessor of job z1?</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>Is job 9 predecessor of job s1?</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>Is job 9 predecessor of job s2?</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>Is job 10 predecessor of job z2?</t>
+        </is>
+      </c>
+      <c r="B162" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>Is job 10 predecessor of job 1?</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>Is job 10 predecessor of job 2?</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>Is job 10 predecessor of job 3?</t>
+        </is>
+      </c>
+      <c r="B165" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>Is job 10 predecessor of job 4?</t>
+        </is>
+      </c>
+      <c r="B166" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>Is job 10 predecessor of job 5?</t>
+        </is>
+      </c>
+      <c r="B167" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>Is job 10 predecessor of job 6?</t>
+        </is>
+      </c>
+      <c r="B168" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>Is job 10 predecessor of job 7?</t>
+        </is>
+      </c>
+      <c r="B169" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>Is job 10 predecessor of job 8?</t>
+        </is>
+      </c>
+      <c r="B170" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>Is job 10 predecessor of job 9?</t>
+        </is>
+      </c>
+      <c r="B171" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>Is job 10 predecessor of job 10?</t>
+        </is>
+      </c>
+      <c r="B172" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>Is job 10 predecessor of job 11?</t>
+        </is>
+      </c>
+      <c r="B173" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>Is job 10 predecessor of job 12?</t>
+        </is>
+      </c>
+      <c r="B174" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>Is job 10 predecessor of job z1?</t>
+        </is>
+      </c>
+      <c r="B175" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>Is job 10 predecessor of job s1?</t>
+        </is>
+      </c>
+      <c r="B176" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>Is job 10 predecessor of job s2?</t>
+        </is>
+      </c>
+      <c r="B177" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>Is job 11 predecessor of job z2?</t>
+        </is>
+      </c>
+      <c r="B178" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>Is job 11 predecessor of job 1?</t>
+        </is>
+      </c>
+      <c r="B179" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>Is job 11 predecessor of job 2?</t>
+        </is>
+      </c>
+      <c r="B180" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>Is job 11 predecessor of job 3?</t>
+        </is>
+      </c>
+      <c r="B181" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>Is job 11 predecessor of job 4?</t>
+        </is>
+      </c>
+      <c r="B182" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>Is job 11 predecessor of job 5?</t>
+        </is>
+      </c>
+      <c r="B183" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>Is job 11 predecessor of job 6?</t>
+        </is>
+      </c>
+      <c r="B184" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>Is job 11 predecessor of job 7?</t>
+        </is>
+      </c>
+      <c r="B185" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>Is job 11 predecessor of job 8?</t>
+        </is>
+      </c>
+      <c r="B186" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>Is job 11 predecessor of job 9?</t>
+        </is>
+      </c>
+      <c r="B187" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>Is job 11 predecessor of job 10?</t>
+        </is>
+      </c>
+      <c r="B188" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>Is job 11 predecessor of job 11?</t>
+        </is>
+      </c>
+      <c r="B189" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>Is job 11 predecessor of job 12?</t>
+        </is>
+      </c>
+      <c r="B190" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>Is job 11 predecessor of job z1?</t>
+        </is>
+      </c>
+      <c r="B191" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>Is job 11 predecessor of job s1?</t>
+        </is>
+      </c>
+      <c r="B192" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>Is job 11 predecessor of job s2?</t>
+        </is>
+      </c>
+      <c r="B193" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>Is job 12 predecessor of job z2?</t>
+        </is>
+      </c>
+      <c r="B194" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>Is job 12 predecessor of job 1?</t>
+        </is>
+      </c>
+      <c r="B195" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>Is job 12 predecessor of job 2?</t>
+        </is>
+      </c>
+      <c r="B196" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>Is job 12 predecessor of job 3?</t>
+        </is>
+      </c>
+      <c r="B197" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>Is job 12 predecessor of job 4?</t>
+        </is>
+      </c>
+      <c r="B198" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>Is job 12 predecessor of job 5?</t>
+        </is>
+      </c>
+      <c r="B199" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>Is job 12 predecessor of job 6?</t>
+        </is>
+      </c>
+      <c r="B200" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>Is job 12 predecessor of job 7?</t>
+        </is>
+      </c>
+      <c r="B201" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>Is job 12 predecessor of job 8?</t>
+        </is>
+      </c>
+      <c r="B202" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>Is job 12 predecessor of job 9?</t>
+        </is>
+      </c>
+      <c r="B203" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>Is job 12 predecessor of job 10?</t>
+        </is>
+      </c>
+      <c r="B204" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>Is job 12 predecessor of job 11?</t>
+        </is>
+      </c>
+      <c r="B205" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>Is job 12 predecessor of job 12?</t>
+        </is>
+      </c>
+      <c r="B206" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>Is job 12 predecessor of job z1?</t>
+        </is>
+      </c>
+      <c r="B207" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>Is job 12 predecessor of job s1?</t>
+        </is>
+      </c>
+      <c r="B208" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>Is job 12 predecessor of job s2?</t>
+        </is>
+      </c>
+      <c r="B209" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>Is job z1 predecessor of job z2?</t>
+        </is>
+      </c>
+      <c r="B210" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>Is job z1 predecessor of job 1?</t>
+        </is>
+      </c>
+      <c r="B211" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>Is job z1 predecessor of job 2?</t>
+        </is>
+      </c>
+      <c r="B212" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>Is job z1 predecessor of job 3?</t>
+        </is>
+      </c>
+      <c r="B213" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>Is job z1 predecessor of job 4?</t>
+        </is>
+      </c>
+      <c r="B214" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>Is job z1 predecessor of job 5?</t>
+        </is>
+      </c>
+      <c r="B215" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>Is job z1 predecessor of job 6?</t>
+        </is>
+      </c>
+      <c r="B216" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>Is job z1 predecessor of job 7?</t>
+        </is>
+      </c>
+      <c r="B217" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>Is job z1 predecessor of job 8?</t>
+        </is>
+      </c>
+      <c r="B218" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>Is job z1 predecessor of job 9?</t>
+        </is>
+      </c>
+      <c r="B219" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>Is job z1 predecessor of job 10?</t>
+        </is>
+      </c>
+      <c r="B220" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>Is job z1 predecessor of job 11?</t>
+        </is>
+      </c>
+      <c r="B221" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>Is job z1 predecessor of job 12?</t>
+        </is>
+      </c>
+      <c r="B222" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>Is job z1 predecessor of job z1?</t>
+        </is>
+      </c>
+      <c r="B223" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>Is job z1 predecessor of job s1?</t>
+        </is>
+      </c>
+      <c r="B224" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>Is job z1 predecessor of job s2?</t>
+        </is>
+      </c>
+      <c r="B225" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>Is job s1 predecessor of job z2?</t>
+        </is>
+      </c>
+      <c r="B226" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>Is job s1 predecessor of job 1?</t>
+        </is>
+      </c>
+      <c r="B227" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>Is job s1 predecessor of job 2?</t>
+        </is>
+      </c>
+      <c r="B228" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>Is job s1 predecessor of job 3?</t>
+        </is>
+      </c>
+      <c r="B229" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>Is job s1 predecessor of job 4?</t>
+        </is>
+      </c>
+      <c r="B230" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>Is job s1 predecessor of job 5?</t>
+        </is>
+      </c>
+      <c r="B231" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>Is job s1 predecessor of job 6?</t>
+        </is>
+      </c>
+      <c r="B232" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>Is job s1 predecessor of job 7?</t>
+        </is>
+      </c>
+      <c r="B233" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>Is job s1 predecessor of job 8?</t>
+        </is>
+      </c>
+      <c r="B234" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>Is job s1 predecessor of job 9?</t>
+        </is>
+      </c>
+      <c r="B235" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>Is job s1 predecessor of job 10?</t>
+        </is>
+      </c>
+      <c r="B236" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>Is job s1 predecessor of job 11?</t>
+        </is>
+      </c>
+      <c r="B237" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>Is job s1 predecessor of job 12?</t>
+        </is>
+      </c>
+      <c r="B238" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>Is job s1 predecessor of job z1?</t>
+        </is>
+      </c>
+      <c r="B239" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>Is job s1 predecessor of job s1?</t>
+        </is>
+      </c>
+      <c r="B240" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>Is job s1 predecessor of job s2?</t>
+        </is>
+      </c>
+      <c r="B241" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>Is job s2 predecessor of job z2?</t>
+        </is>
+      </c>
+      <c r="B242" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>Is job s2 predecessor of job 1?</t>
+        </is>
+      </c>
+      <c r="B243" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>Is job s2 predecessor of job 2?</t>
+        </is>
+      </c>
+      <c r="B244" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>Is job s2 predecessor of job 3?</t>
+        </is>
+      </c>
+      <c r="B245" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>Is job s2 predecessor of job 4?</t>
+        </is>
+      </c>
+      <c r="B246" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>Is job s2 predecessor of job 5?</t>
+        </is>
+      </c>
+      <c r="B247" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>Is job s2 predecessor of job 6?</t>
+        </is>
+      </c>
+      <c r="B248" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>Is job s2 predecessor of job 7?</t>
+        </is>
+      </c>
+      <c r="B249" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>Is job s2 predecessor of job 8?</t>
+        </is>
+      </c>
+      <c r="B250" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>Is job s2 predecessor of job 9?</t>
+        </is>
+      </c>
+      <c r="B251" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>Is job s2 predecessor of job 10?</t>
+        </is>
+      </c>
+      <c r="B252" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>Is job s2 predecessor of job 11?</t>
+        </is>
+      </c>
+      <c r="B253" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>Is job s2 predecessor of job 12?</t>
+        </is>
+      </c>
+      <c r="B254" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>Is job s2 predecessor of job z1?</t>
+        </is>
+      </c>
+      <c r="B255" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>Is job s2 predecessor of job s1?</t>
+        </is>
+      </c>
+      <c r="B256" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>Is job s2 predecessor of job s2?</t>
+        </is>
+      </c>
+      <c r="B257" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>Job z2 is executed by machine:</t>
+        </is>
+      </c>
+      <c r="B258" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>Job 1 is executed by machine:</t>
+        </is>
+      </c>
+      <c r="B259" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>Job 2 is executed by machine:</t>
+        </is>
+      </c>
+      <c r="B260" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>Job 3 is executed by machine:</t>
+        </is>
+      </c>
+      <c r="B261" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>Job 4 is executed by machine:</t>
+        </is>
+      </c>
+      <c r="B262" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>Job 5 is executed by machine:</t>
+        </is>
+      </c>
+      <c r="B263" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>Job 6 is executed by machine:</t>
+        </is>
+      </c>
+      <c r="B264" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>Job 7 is executed by machine:</t>
+        </is>
+      </c>
+      <c r="B265" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>Job 8 is executed by machine:</t>
+        </is>
+      </c>
+      <c r="B266" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>Job 9 is executed by machine:</t>
+        </is>
+      </c>
+      <c r="B267" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>Job 10 is executed by machine:</t>
+        </is>
+      </c>
+      <c r="B268" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>Job 11 is executed by machine:</t>
+        </is>
+      </c>
+      <c r="B269" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>Job 12 is executed by machine:</t>
+        </is>
+      </c>
+      <c r="B270" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>Job z1 is executed by machine:</t>
+        </is>
+      </c>
+      <c r="B271" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>Job s1 is executed by machine:</t>
+        </is>
+      </c>
+      <c r="B272" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>Job s2 is executed by machine:</t>
+        </is>
+      </c>
+      <c r="B273" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>Job z2 is executed on day:</t>
+        </is>
+      </c>
+      <c r="B274" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>Job 1 is executed on day:</t>
+        </is>
+      </c>
+      <c r="B275" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>Job 2 is executed on day:</t>
+        </is>
+      </c>
+      <c r="B276" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>Job 3 is executed on day:</t>
+        </is>
+      </c>
+      <c r="B277" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>Job 4 is executed on day:</t>
+        </is>
+      </c>
+      <c r="B278" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>Job 5 is executed on day:</t>
+        </is>
+      </c>
+      <c r="B279" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>Job 6 is executed on day:</t>
+        </is>
+      </c>
+      <c r="B280" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>Job 7 is executed on day:</t>
+        </is>
+      </c>
+      <c r="B281" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>Job 8 is executed on day:</t>
+        </is>
+      </c>
+      <c r="B282" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>Job 9 is executed on day:</t>
+        </is>
+      </c>
+      <c r="B283" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>Job 10 is executed on day:</t>
+        </is>
+      </c>
+      <c r="B284" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>Job 11 is executed on day:</t>
+        </is>
+      </c>
+      <c r="B285" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>Job 12 is executed on day:</t>
+        </is>
+      </c>
+      <c r="B286" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>Job z1 is executed on day:</t>
+        </is>
+      </c>
+      <c r="B287" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>Job s1 is executed on day:</t>
+        </is>
+      </c>
+      <c r="B288" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>Job s2 is executed on day:</t>
+        </is>
+      </c>
+      <c r="B289" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>Job z2 is executed on minute:</t>
+        </is>
+      </c>
+      <c r="B290" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>Job 1 is executed on minute:</t>
+        </is>
+      </c>
+      <c r="B291" t="n">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>Job 2 is executed on minute:</t>
+        </is>
+      </c>
+      <c r="B292" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>Job 3 is executed on minute:</t>
+        </is>
+      </c>
+      <c r="B293" t="n">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>Job 4 is executed on minute:</t>
+        </is>
+      </c>
+      <c r="B294" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>Job 5 is executed on minute:</t>
+        </is>
+      </c>
+      <c r="B295" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>Job 6 is executed on minute:</t>
+        </is>
+      </c>
+      <c r="B296" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>Job 7 is executed on minute:</t>
+        </is>
+      </c>
+      <c r="B297" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>Job 8 is executed on minute:</t>
+        </is>
+      </c>
+      <c r="B298" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>Job 9 is executed on minute:</t>
+        </is>
+      </c>
+      <c r="B299" t="n">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>Job 10 is executed on minute:</t>
+        </is>
+      </c>
+      <c r="B300" t="n">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>Job 11 is executed on minute:</t>
+        </is>
+      </c>
+      <c r="B301" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>Job 12 is executed on minute:</t>
+        </is>
+      </c>
+      <c r="B302" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>Job z1 is executed on minute:</t>
+        </is>
+      </c>
+      <c r="B303" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
           <t>Job s1 is executed on minute:</t>
         </is>
       </c>
-      <c r="B41" t="n">
+      <c r="B304" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>Job s2 is executed on minute:</t>
+        </is>
+      </c>
+      <c r="B305" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>